<commit_message>
Commit Semanal (CW 48)
</commit_message>
<xml_diff>
--- a/CODIGO-FONTE/Monografia/RURUCAg.xlsx
+++ b/CODIGO-FONTE/Monografia/RURUCAg.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11880" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11880"/>
   </bookViews>
   <sheets>
     <sheet name="Voters" sheetId="1" r:id="rId1"/>
@@ -24,12 +24,11 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Session 1'!$A$1:$B$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1135" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1087" uniqueCount="338">
   <si>
     <t>Date</t>
   </si>
@@ -4300,8 +4299,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:AK23"/>
   <sheetViews>
-    <sheetView showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="Z3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AG19" sqref="AG19"/>
+    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="M3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AI24" sqref="AI24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4320,7 +4319,9 @@
     <col min="31" max="31" width="30.875" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="31.125" customWidth="1"/>
     <col min="33" max="33" width="30.375" customWidth="1"/>
-    <col min="34" max="36" width="5.625" customWidth="1"/>
+    <col min="34" max="34" width="5.625" customWidth="1"/>
+    <col min="35" max="35" width="35.5" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="5.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:37" ht="45" x14ac:dyDescent="0.25">
@@ -4531,14 +4532,14 @@
       <c r="AG4" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="AH4" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="AI4" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="AJ4" s="35" t="s">
-        <v>41</v>
+      <c r="AH4" s="35">
+        <v>1</v>
+      </c>
+      <c r="AI4" s="35">
+        <v>1</v>
+      </c>
+      <c r="AJ4" s="35">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:37" s="35" customFormat="1" x14ac:dyDescent="0.2">
@@ -4641,14 +4642,14 @@
       <c r="AG5" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="AH5" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="AI5" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="AJ5" s="35" t="s">
-        <v>41</v>
+      <c r="AH5" s="35">
+        <v>1</v>
+      </c>
+      <c r="AI5" s="35">
+        <v>1</v>
+      </c>
+      <c r="AJ5" s="35">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:37" s="35" customFormat="1" x14ac:dyDescent="0.2">
@@ -4751,14 +4752,14 @@
       <c r="AG6" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="AH6" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="AI6" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="AJ6" s="35" t="s">
-        <v>41</v>
+      <c r="AH6" s="35">
+        <v>1</v>
+      </c>
+      <c r="AI6" s="35">
+        <v>1</v>
+      </c>
+      <c r="AJ6" s="35">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:37" s="35" customFormat="1" x14ac:dyDescent="0.2">
@@ -4861,14 +4862,14 @@
       <c r="AG7" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="AH7" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="AI7" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="AJ7" s="35" t="s">
-        <v>41</v>
+      <c r="AH7" s="35">
+        <v>1</v>
+      </c>
+      <c r="AI7" s="35">
+        <v>1</v>
+      </c>
+      <c r="AJ7" s="35">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:37" s="35" customFormat="1" x14ac:dyDescent="0.2">
@@ -4968,14 +4969,14 @@
       <c r="AF8" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="AH8" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="AI8" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="AJ8" s="35" t="s">
-        <v>41</v>
+      <c r="AH8" s="35">
+        <v>1</v>
+      </c>
+      <c r="AI8" s="35">
+        <v>1</v>
+      </c>
+      <c r="AJ8" s="35">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:37" s="35" customFormat="1" x14ac:dyDescent="0.2">
@@ -5078,14 +5079,14 @@
       <c r="AG9" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="AH9" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="AI9" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="AJ9" s="35" t="s">
-        <v>41</v>
+      <c r="AH9" s="35">
+        <v>1</v>
+      </c>
+      <c r="AI9" s="35">
+        <v>1</v>
+      </c>
+      <c r="AJ9" s="35">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:37" s="35" customFormat="1" x14ac:dyDescent="0.2">
@@ -5188,14 +5189,14 @@
       <c r="AG10" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="AH10" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="AI10" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="AJ10" s="35" t="s">
-        <v>41</v>
+      <c r="AH10" s="35">
+        <v>1</v>
+      </c>
+      <c r="AI10" s="35">
+        <v>1</v>
+      </c>
+      <c r="AJ10" s="35">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:37" s="35" customFormat="1" x14ac:dyDescent="0.2">
@@ -5292,14 +5293,14 @@
       <c r="AE11" s="35">
         <v>2</v>
       </c>
-      <c r="AH11" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="AI11" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="AJ11" s="35" t="s">
-        <v>41</v>
+      <c r="AH11" s="35">
+        <v>1</v>
+      </c>
+      <c r="AI11" s="35">
+        <v>1</v>
+      </c>
+      <c r="AJ11" s="35">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:37" s="35" customFormat="1" x14ac:dyDescent="0.2">
@@ -5402,14 +5403,14 @@
       <c r="AG12" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="AH12" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="AI12" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="AJ12" s="35" t="s">
-        <v>41</v>
+      <c r="AH12" s="35">
+        <v>1</v>
+      </c>
+      <c r="AI12" s="35">
+        <v>1</v>
+      </c>
+      <c r="AJ12" s="35">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:37" s="35" customFormat="1" x14ac:dyDescent="0.2">
@@ -5512,14 +5513,14 @@
       <c r="AG13" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="AH13" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="AI13" s="35" t="s">
-        <v>47</v>
-      </c>
-      <c r="AJ13" s="35" t="s">
-        <v>41</v>
+      <c r="AH13" s="35">
+        <v>1</v>
+      </c>
+      <c r="AI13" s="35">
+        <v>4</v>
+      </c>
+      <c r="AJ13" s="35">
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:37" s="35" customFormat="1" x14ac:dyDescent="0.2">
@@ -5622,14 +5623,14 @@
       <c r="AG14" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="AH14" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="AI14" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="AJ14" s="35" t="s">
-        <v>41</v>
+      <c r="AH14" s="35">
+        <v>1</v>
+      </c>
+      <c r="AI14" s="35">
+        <v>1</v>
+      </c>
+      <c r="AJ14" s="35">
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:37" s="35" customFormat="1" x14ac:dyDescent="0.2">
@@ -5732,14 +5733,14 @@
       <c r="AG15" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="AH15" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="AI15" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="AJ15" s="35" t="s">
-        <v>41</v>
+      <c r="AH15" s="35">
+        <v>1</v>
+      </c>
+      <c r="AI15" s="35">
+        <v>1</v>
+      </c>
+      <c r="AJ15" s="35">
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:37" s="35" customFormat="1" x14ac:dyDescent="0.2">
@@ -5842,14 +5843,14 @@
       <c r="AG16" s="35" t="s">
         <v>97</v>
       </c>
-      <c r="AH16" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="AI16" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="AJ16" s="35" t="s">
-        <v>41</v>
+      <c r="AH16" s="35">
+        <v>1</v>
+      </c>
+      <c r="AI16" s="35">
+        <v>1</v>
+      </c>
+      <c r="AJ16" s="35">
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:36" s="35" customFormat="1" x14ac:dyDescent="0.2">
@@ -5952,14 +5953,14 @@
       <c r="AG17" s="35" t="s">
         <v>100</v>
       </c>
-      <c r="AH17" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="AI17" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="AJ17" s="35" t="s">
-        <v>41</v>
+      <c r="AH17" s="35">
+        <v>1</v>
+      </c>
+      <c r="AI17" s="35">
+        <v>1</v>
+      </c>
+      <c r="AJ17" s="35">
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:36" s="35" customFormat="1" x14ac:dyDescent="0.2">
@@ -6062,14 +6063,14 @@
       <c r="AG18" s="35" t="s">
         <v>103</v>
       </c>
-      <c r="AH18" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="AI18" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="AJ18" s="35" t="s">
-        <v>41</v>
+      <c r="AH18" s="35">
+        <v>1</v>
+      </c>
+      <c r="AI18" s="35">
+        <v>1</v>
+      </c>
+      <c r="AJ18" s="35">
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:36" x14ac:dyDescent="0.2">
@@ -6172,14 +6173,14 @@
       <c r="AG19" t="s">
         <v>106</v>
       </c>
-      <c r="AH19" t="s">
-        <v>41</v>
-      </c>
-      <c r="AI19" t="s">
-        <v>41</v>
-      </c>
-      <c r="AJ19" t="s">
-        <v>41</v>
+      <c r="AH19">
+        <v>1</v>
+      </c>
+      <c r="AI19">
+        <v>1</v>
+      </c>
+      <c r="AJ19">
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:36" x14ac:dyDescent="0.2">
@@ -6195,7 +6196,7 @@
         <v>87.5</v>
       </c>
       <c r="G20" s="16">
-        <f t="shared" ref="G20:AE20" si="0">(100/16*(COUNTIF(G$4:G$19,$D$20)))</f>
+        <f t="shared" ref="G20:AJ20" si="0">(100/16*(COUNTIF(G$4:G$19,$D$20)))</f>
         <v>68.75</v>
       </c>
       <c r="H20" s="16">
@@ -6293,6 +6294,26 @@
       <c r="AE20" s="16">
         <f t="shared" si="0"/>
         <v>75</v>
+      </c>
+      <c r="AF20" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AG20" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AH20" s="16">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="AI20" s="16">
+        <f t="shared" si="0"/>
+        <v>93.75</v>
+      </c>
+      <c r="AJ20" s="16">
+        <f t="shared" si="0"/>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:36" x14ac:dyDescent="0.2">
@@ -11269,8 +11290,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N48"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -12635,7 +12656,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>

</xml_diff>